<commit_message>
updated data for 2018 and 2019
</commit_message>
<xml_diff>
--- a/hate stats.xlsx
+++ b/hate stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agutf\Desktop\Box Sync\2019_2summer\hate crime article\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agutf\Sync\2019_2summer\hate crime article\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655C6B2A-D15E-4C50-852E-7B19A2188205}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F5B43E-0DE5-4287-84A1-A90AB5C11B42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="21864" windowHeight="13152" xr2:uid="{678F45DA-570B-4457-9960-F0AB35FEED8E}"/>
   </bookViews>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Year</t>
   </si>
@@ -165,12 +167,6 @@
     <t>https://www.adl.org/sites/default/files/documents/assets/pdf/press-center/2012-audit-of-anti-semitic-incidents.pdf</t>
   </si>
   <si>
-    <t>property</t>
-  </si>
-  <si>
-    <t>persons</t>
-  </si>
-  <si>
     <t>total</t>
   </si>
   <si>
@@ -181,6 +177,42 @@
   </si>
   <si>
     <t>https://ucr.fbi.gov/hate-crime/1996</t>
+  </si>
+  <si>
+    <t>https://ucr.fbi.gov/hate-crime/2018/topic-pages/tables/table-1.xls</t>
+  </si>
+  <si>
+    <t>https://www.bjs.gov/content/pub/pdf/hcs1317pp.pdf</t>
+  </si>
+  <si>
+    <t>Main site</t>
+  </si>
+  <si>
+    <t>https://www.bjs.gov/index.cfm?ty=pbse&amp;sid=72</t>
+  </si>
+  <si>
+    <t>Digitized data from the figure</t>
+  </si>
+  <si>
+    <t>vandalism</t>
+  </si>
+  <si>
+    <t>harassment, threats, and assualts</t>
+  </si>
+  <si>
+    <t>Data for earlier years</t>
+  </si>
+  <si>
+    <t>Recent data:</t>
+  </si>
+  <si>
+    <t>https://www.adl.org/audit2018</t>
+  </si>
+  <si>
+    <t>https://www.adl.org/media/13144/download</t>
+  </si>
+  <si>
+    <t>In 2019 reported (data might be incomplete - retrieved 1/5)</t>
   </si>
 </sst>
 </file>
@@ -191,7 +223,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +280,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,7 +311,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -287,6 +327,7 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -363,10 +404,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>ALL!$A$2:$A$30</c:f>
+              <c:f>ALL!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>1990</c:v>
                 </c:pt>
@@ -453,16 +494,22 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2020</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ALL!$B$2:$B$30</c:f>
+              <c:f>ALL!$B$2:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>1691.06165545048</c:v>
                 </c:pt>
@@ -549,6 +596,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>1879</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -585,10 +635,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>ALL!$A$2:$A$30</c:f>
+              <c:f>ALL!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>1990</c:v>
                 </c:pt>
@@ -675,6 +725,12 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2020</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -685,7 +741,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
-                <c:pt idx="6">
+                <c:pt idx="6" formatCode="#,##0">
                   <c:v>1109</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="#,##0">
@@ -715,41 +771,44 @@
                 <c:pt idx="15">
                   <c:v>848</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="16" formatCode="#,##0">
                   <c:v>967</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="17" formatCode="#,##0">
                   <c:v>969</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="#,##0">
                   <c:v>1013</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="19" formatCode="#,##0">
                   <c:v>931</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="20" formatCode="#,##0">
                   <c:v>887</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="21" formatCode="#,##0">
                   <c:v>771</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="22" formatCode="#,##0">
                   <c:v>674</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="23" formatCode="#,##0">
                   <c:v>625</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="24" formatCode="#,##0">
                   <c:v>609</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="25" formatCode="#,##0">
                   <c:v>664</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="26" formatCode="#,##0">
                   <c:v>684</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="27" formatCode="#,##0">
                   <c:v>938</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="#,##0">
+                  <c:v>835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1984,23 +2043,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>15621</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314518</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>371439</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>156757</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>158093</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72313D96-A7D1-4A49-A9B4-ED5B5EDE61FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D3100C1-5992-4183-9BFA-FB0D33C3DEE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2016,8 +2075,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12893040" y="564261"/>
-          <a:ext cx="4120479" cy="2884336"/>
+          <a:off x="7995478" y="3569971"/>
+          <a:ext cx="8164615" cy="4728210"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2028,23 +2087,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>78298</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>422910</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>561953</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>87631</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>62829</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>72556</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D3100C1-5992-4183-9BFA-FB0D33C3DEE7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D85E731-508B-4647-9BE5-7B4D6060AFD5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2060,8 +2119,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9039418" y="3589021"/>
-          <a:ext cx="8164615" cy="4728210"/>
+          <a:off x="2983230" y="7612380"/>
+          <a:ext cx="4120479" cy="2884336"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2126,16 +2185,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>25111</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>120361</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>354733</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>28631</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>331873</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>123881</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2158,7 +2217,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4381500" y="207991"/>
+          <a:off x="4998720" y="1400521"/>
           <a:ext cx="8774833" cy="4758400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2470,8 +2529,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94352461-44A9-40DA-9CD6-845A323A112B}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2496,7 +2558,7 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2554,10 +2616,12 @@
       <c r="B8">
         <v>1723.9010634286899</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="5">
+        <f>FBI!B2</f>
         <v>8759</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
+        <f>FBI!C2</f>
         <v>1109</v>
       </c>
     </row>
@@ -2718,10 +2782,12 @@
       <c r="C18" s="2">
         <v>230490</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
+        <f>FBI!B12</f>
         <v>7722</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
+        <f>FBI!C12</f>
         <v>967</v>
       </c>
       <c r="F18" s="3"/>
@@ -2737,10 +2803,12 @@
       <c r="C19" s="2">
         <v>263440</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="5">
+        <f>FBI!B13</f>
         <v>7624</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="5">
+        <f>FBI!C13</f>
         <v>969</v>
       </c>
       <c r="F19" s="3"/>
@@ -2756,10 +2824,12 @@
       <c r="C20" s="2">
         <v>266640</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="5">
+        <f>FBI!B14</f>
         <v>7783</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="5">
+        <f>FBI!C14</f>
         <v>1013</v>
       </c>
       <c r="F20" s="3"/>
@@ -2775,10 +2845,12 @@
       <c r="C21" s="2">
         <v>284620</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="5">
+        <f>FBI!B15</f>
         <v>6604</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="5">
+        <f>FBI!C15</f>
         <v>931</v>
       </c>
       <c r="F21" s="3"/>
@@ -2794,10 +2866,12 @@
       <c r="C22" s="2">
         <v>273100</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="5">
+        <f>FBI!B16</f>
         <v>6628</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="5">
+        <f>FBI!C16</f>
         <v>887</v>
       </c>
       <c r="F22" s="3"/>
@@ -2813,10 +2887,12 @@
       <c r="C23" s="2">
         <v>218010</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="5">
+        <f>FBI!B17</f>
         <v>6222</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="5">
+        <f>FBI!C17</f>
         <v>771</v>
       </c>
       <c r="F23" s="3"/>
@@ -2832,10 +2908,12 @@
       <c r="C24" s="2">
         <v>293790</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="5">
+        <f>FBI!B18</f>
         <v>5796</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="5">
+        <f>FBI!C18</f>
         <v>674</v>
       </c>
       <c r="F24" s="3"/>
@@ -2852,10 +2930,12 @@
       <c r="C25" s="2">
         <v>272420</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="5">
+        <f>FBI!B19</f>
         <v>5928</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="5">
+        <f>FBI!C19</f>
         <v>625</v>
       </c>
       <c r="F25" s="3"/>
@@ -2871,10 +2951,12 @@
       <c r="C26" s="2">
         <v>215010</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="5">
+        <f>FBI!B20</f>
         <v>5479</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="5">
+        <f>FBI!C20</f>
         <v>609</v>
       </c>
       <c r="F26" s="3"/>
@@ -2890,10 +2972,12 @@
       <c r="C27" s="2">
         <v>207880</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="5">
+        <f>FBI!B21</f>
         <v>5850</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="5">
+        <f>FBI!C21</f>
         <v>664</v>
       </c>
       <c r="F27" s="3"/>
@@ -2909,10 +2993,12 @@
       <c r="C28" s="2">
         <v>196769</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="5">
+        <f>FBI!B22</f>
         <v>6121</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="5">
+        <f>FBI!C22</f>
         <v>684</v>
       </c>
       <c r="F28" s="3"/>
@@ -2928,10 +3014,12 @@
       <c r="C29" s="2">
         <v>194662</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="5">
+        <f>FBI!B23</f>
         <v>7175</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="5">
+        <f>FBI!C23</f>
         <v>938</v>
       </c>
       <c r="F29" s="3"/>
@@ -2944,22 +3032,37 @@
       <c r="B30">
         <v>1879</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="D30" s="5">
+        <f>FBI!B24</f>
+        <v>7120</v>
+      </c>
+      <c r="E30" s="5">
+        <f>FBI!C24</f>
+        <v>835</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>2019</v>
       </c>
+      <c r="B31">
+        <v>1347</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>2020</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>2021</v>
+      </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
@@ -2971,332 +3074,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B128050-D099-4CF3-980A-52E80A59B07F}">
-  <dimension ref="B2:AD49"/>
+  <dimension ref="B4:Z76"/>
   <sheetViews>
-    <sheetView topLeftCell="O10" workbookViewId="0">
-      <selection activeCell="AD21" sqref="AD21"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="2" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="O2" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB4">
-        <v>1978.9630023683301</v>
-      </c>
-      <c r="AC4">
-        <f>ROUND(AB4, 0)</f>
-        <v>1979</v>
-      </c>
-      <c r="AD4">
-        <v>123.42108298600201</v>
-      </c>
-    </row>
-    <row r="5" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB5">
-        <v>1979.9835382604199</v>
-      </c>
-      <c r="AC5">
-        <f t="shared" ref="AC5:AC37" si="0">ROUND(AB5, 0)</f>
-        <v>1980</v>
-      </c>
-      <c r="AD5">
-        <v>482.007619775607</v>
-      </c>
-    </row>
-    <row r="6" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB6">
-        <v>1980.94793225068</v>
-      </c>
-      <c r="AC6">
-        <f t="shared" si="0"/>
-        <v>1981</v>
-      </c>
-      <c r="AD6">
-        <v>1322.0852981026301</v>
-      </c>
-    </row>
-    <row r="7" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB7">
-        <v>1981.9711509602701</v>
-      </c>
-      <c r="AC7">
-        <f t="shared" si="0"/>
-        <v>1982</v>
-      </c>
-      <c r="AD7">
-        <v>1418.7312884238199</v>
-      </c>
-    </row>
-    <row r="8" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB8">
-        <v>1982.9737751001201</v>
-      </c>
-      <c r="AC8">
-        <f t="shared" si="0"/>
-        <v>1983</v>
-      </c>
-      <c r="AD8">
-        <v>1026.1561795760399</v>
-      </c>
-    </row>
-    <row r="9" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB9">
-        <v>1983.9718226689099</v>
-      </c>
-      <c r="AC9">
-        <f t="shared" si="0"/>
-        <v>1984</v>
-      </c>
-      <c r="AD9">
-        <v>1080.4208264684701</v>
-      </c>
-    </row>
-    <row r="10" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB10">
-        <v>1985.02297424323</v>
-      </c>
-      <c r="AC10">
-        <f t="shared" si="0"/>
-        <v>1985</v>
-      </c>
-      <c r="AD10">
-        <v>949.80348003036897</v>
-      </c>
-    </row>
-    <row r="11" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB11">
-        <v>1985.97087679641</v>
-      </c>
-      <c r="AC11">
-        <f t="shared" si="0"/>
-        <v>1986</v>
-      </c>
-      <c r="AD11">
-        <v>900.04510576613495</v>
-      </c>
-    </row>
-    <row r="12" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB12">
-        <v>1986.9682142076199</v>
-      </c>
-      <c r="AC12">
-        <f t="shared" si="0"/>
-        <v>1987</v>
-      </c>
-      <c r="AD12">
-        <v>1023.6469561355</v>
-      </c>
-    </row>
-    <row r="13" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB13">
-        <v>1987.98981533607</v>
-      </c>
-      <c r="AC13">
-        <f t="shared" si="0"/>
-        <v>1988</v>
-      </c>
-      <c r="AD13">
-        <v>1278.2276877097099</v>
-      </c>
-    </row>
-    <row r="14" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB14">
-        <v>1989.01248170088</v>
-      </c>
-      <c r="AC14">
-        <f t="shared" si="0"/>
-        <v>1989</v>
-      </c>
-      <c r="AD14">
-        <v>1428.8026140685199</v>
-      </c>
-    </row>
-    <row r="15" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB15">
-        <v>1989.95718854497</v>
-      </c>
-      <c r="AC15">
-        <f t="shared" si="0"/>
-        <v>1990</v>
-      </c>
-      <c r="AD15">
-        <v>1691.06165545048</v>
-      </c>
-    </row>
-    <row r="16" spans="15:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB16">
-        <v>1990.9538157986101</v>
-      </c>
-      <c r="AC16">
-        <f t="shared" si="0"/>
-        <v>1991</v>
-      </c>
-      <c r="AD16">
-        <v>1884.0007092967801</v>
-      </c>
-    </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB17">
-        <v>1991.97952005972</v>
-      </c>
-      <c r="AC17">
-        <f t="shared" si="0"/>
-        <v>1992</v>
-      </c>
-      <c r="AD17">
-        <v>1737.96648744871</v>
-      </c>
-    </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB18">
-        <v>1992.9767391113401</v>
-      </c>
-      <c r="AC18">
-        <f t="shared" si="0"/>
-        <v>1993</v>
-      </c>
-      <c r="AD18">
-        <v>1873.1245383975699</v>
-      </c>
-    </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB19">
-        <v>1993.9990109441701</v>
-      </c>
-      <c r="AC19">
-        <f t="shared" si="0"/>
-        <v>1994</v>
-      </c>
-      <c r="AD19">
-        <v>2062.22013335468</v>
-      </c>
-    </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB20">
-        <v>1994.9485705316999</v>
-      </c>
-      <c r="AC20">
-        <f t="shared" si="0"/>
-        <v>1995</v>
-      </c>
-      <c r="AD20">
-        <v>1850.6749509776</v>
-      </c>
-    </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB21">
-        <v>1995.9740775268201</v>
-      </c>
-      <c r="AC21">
-        <f t="shared" si="0"/>
-        <v>1996</v>
-      </c>
-      <c r="AD21">
-        <v>1723.9010634286899</v>
-      </c>
-    </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB22">
-        <v>1996.9742161151501</v>
-      </c>
-      <c r="AC22">
-        <f t="shared" si="0"/>
-        <v>1997</v>
-      </c>
-      <c r="AD22">
-        <v>1574.00616675016</v>
-      </c>
-    </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB23">
-        <v>1997.99798716953</v>
-      </c>
-      <c r="AC23">
-        <f t="shared" si="0"/>
-        <v>1998</v>
-      </c>
-      <c r="AD23">
-        <v>1616.7232210337399</v>
-      </c>
-    </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB24">
-        <v>1998.97165266149</v>
-      </c>
-      <c r="AC24">
-        <f t="shared" si="0"/>
-        <v>1999</v>
-      </c>
-      <c r="AD24">
-        <v>1551.5651873008301</v>
-      </c>
-    </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB25">
-        <v>1999.9441345575001</v>
-      </c>
-      <c r="AC25">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="AD25">
-        <v>1601.9691593627999</v>
-      </c>
-    </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB26">
-        <v>2000.9956412106001</v>
-      </c>
-      <c r="AC26">
-        <f t="shared" si="0"/>
-        <v>2001</v>
-      </c>
-      <c r="AD26">
-        <v>1436.68321118623</v>
-      </c>
-    </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB27">
-        <v>2001.94176836983</v>
-      </c>
-      <c r="AC27">
-        <f t="shared" si="0"/>
-        <v>2002</v>
-      </c>
-      <c r="AD27">
-        <v>1560.2678456143201</v>
-      </c>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB28">
-        <v>2002.99161798859</v>
-      </c>
-      <c r="AC28">
-        <f t="shared" si="0"/>
-        <v>2003</v>
-      </c>
-      <c r="AD28">
-        <v>1556.7687055505901</v>
-      </c>
-    </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB29">
-        <v>2003.96181159906</v>
-      </c>
-      <c r="AC29">
-        <f t="shared" si="0"/>
-        <v>2004</v>
-      </c>
-      <c r="AD29">
-        <v>1830.5925554826699</v>
-      </c>
-    </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="15:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="O4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="15:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="O5" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="15:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="O7" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B30">
         <v>1211</v>
       </c>
@@ -3327,109 +3128,98 @@
       <c r="K30">
         <v>1879</v>
       </c>
-      <c r="AB30">
-        <v>2004.98672679621</v>
-      </c>
-      <c r="AC30">
-        <f t="shared" si="0"/>
-        <v>2005</v>
-      </c>
-      <c r="AD30">
-        <v>1761.5996708312</v>
-      </c>
-    </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB31">
-        <v>2005.98741772932</v>
-      </c>
-      <c r="AC31">
-        <f t="shared" si="0"/>
-        <v>2006</v>
-      </c>
-      <c r="AD31">
-        <v>1557.77583811506</v>
-      </c>
-    </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB32">
-        <v>2006.9870434260599</v>
-      </c>
-      <c r="AC32">
-        <f t="shared" si="0"/>
-        <v>2007</v>
-      </c>
-      <c r="AD32">
-        <v>1457.9578106143099</v>
-      </c>
-    </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB33">
-        <v>2007.9866296696</v>
-      </c>
-      <c r="AC33">
-        <f t="shared" si="0"/>
-        <v>2008</v>
-      </c>
-      <c r="AD33">
-        <v>1361.9918499733999</v>
-      </c>
-    </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB34">
-        <v>2008.9866498983299</v>
-      </c>
-      <c r="AC34">
-        <f t="shared" si="0"/>
-        <v>2009</v>
-      </c>
-      <c r="AD34">
-        <v>1223.65315387436</v>
-      </c>
-    </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB35">
-        <v>2009.98501309272</v>
-      </c>
-      <c r="AC35">
-        <f t="shared" si="0"/>
-        <v>2010</v>
-      </c>
-      <c r="AD35">
-        <v>1247.10126588816</v>
-      </c>
-    </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB36">
-        <v>2011.0108751666301</v>
-      </c>
-      <c r="AC36">
-        <f t="shared" si="0"/>
-        <v>2011</v>
-      </c>
-      <c r="AD36">
-        <v>1085.6587766007799</v>
-      </c>
-    </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="AB37">
-        <v>2011.98544808217</v>
-      </c>
-      <c r="AC37">
-        <f t="shared" si="0"/>
-        <v>2012</v>
-      </c>
-      <c r="AD37">
-        <v>931.90320509178696</v>
-      </c>
-    </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="33" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="39" spans="2:26" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="2:30" x14ac:dyDescent="0.55000000000000004">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="F40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="F41" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43">
+        <v>1978.9630023683301</v>
+      </c>
+      <c r="C43">
+        <f>ROUND(B43, 0)</f>
+        <v>1979</v>
+      </c>
+      <c r="D43">
+        <v>123.42108298600201</v>
+      </c>
+    </row>
+    <row r="44" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44">
+        <v>1979.9835382604199</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ref="C44:C76" si="0">ROUND(B44, 0)</f>
+        <v>1980</v>
+      </c>
+      <c r="D44">
+        <v>482.007619775607</v>
+      </c>
+    </row>
+    <row r="45" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45">
+        <v>1980.94793225068</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>1981</v>
+      </c>
+      <c r="D45">
+        <v>1322.0852981026301</v>
+      </c>
+    </row>
+    <row r="46" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46">
+        <v>1981.9711509602701</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>1982</v>
+      </c>
+      <c r="D46">
+        <v>1418.7312884238199</v>
+      </c>
+    </row>
+    <row r="47" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47">
+        <v>1982.9737751001201</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>1983</v>
+      </c>
+      <c r="D47">
+        <v>1026.1561795760399</v>
+      </c>
       <c r="O47" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="P47">
         <v>531</v>
@@ -3465,9 +3255,19 @@
         <v>440</v>
       </c>
     </row>
-    <row r="48" spans="2:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48">
+        <v>1983.9718226689099</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>1984</v>
+      </c>
+      <c r="D48">
+        <v>1080.4208264684701</v>
+      </c>
       <c r="O48" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="P48">
         <v>1028</v>
@@ -3503,9 +3303,19 @@
         <v>487</v>
       </c>
     </row>
-    <row r="49" spans="15:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49">
+        <v>1985.02297424323</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>1985</v>
+      </c>
+      <c r="D49">
+        <v>949.80348003036897</v>
+      </c>
       <c r="O49" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P49">
         <f>SUM(P47:P48)</f>
@@ -3552,21 +3362,347 @@
         <v>927</v>
       </c>
     </row>
+    <row r="50" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50">
+        <v>1985.97087679641</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>1986</v>
+      </c>
+      <c r="D50">
+        <v>900.04510576613495</v>
+      </c>
+    </row>
+    <row r="51" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51">
+        <v>1986.9682142076199</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>1987</v>
+      </c>
+      <c r="D51">
+        <v>1023.6469561355</v>
+      </c>
+    </row>
+    <row r="52" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52">
+        <v>1987.98981533607</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>1988</v>
+      </c>
+      <c r="D52">
+        <v>1278.2276877097099</v>
+      </c>
+    </row>
+    <row r="53" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53">
+        <v>1989.01248170088</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>1989</v>
+      </c>
+      <c r="D53">
+        <v>1428.8026140685199</v>
+      </c>
+    </row>
+    <row r="54" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54">
+        <v>1989.95718854497</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>1990</v>
+      </c>
+      <c r="D54">
+        <v>1691.06165545048</v>
+      </c>
+    </row>
+    <row r="55" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55">
+        <v>1990.9538157986101</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>1991</v>
+      </c>
+      <c r="D55">
+        <v>1884.0007092967801</v>
+      </c>
+    </row>
+    <row r="56" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56">
+        <v>1991.97952005972</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>1992</v>
+      </c>
+      <c r="D56">
+        <v>1737.96648744871</v>
+      </c>
+    </row>
+    <row r="57" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57">
+        <v>1992.9767391113401</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>1993</v>
+      </c>
+      <c r="D57">
+        <v>1873.1245383975699</v>
+      </c>
+    </row>
+    <row r="58" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58">
+        <v>1993.9990109441701</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>1994</v>
+      </c>
+      <c r="D58">
+        <v>2062.22013335468</v>
+      </c>
+    </row>
+    <row r="59" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59">
+        <v>1994.9485705316999</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>1995</v>
+      </c>
+      <c r="D59">
+        <v>1850.6749509776</v>
+      </c>
+    </row>
+    <row r="60" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60">
+        <v>1995.9740775268201</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>1996</v>
+      </c>
+      <c r="D60">
+        <v>1723.9010634286899</v>
+      </c>
+    </row>
+    <row r="61" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B61">
+        <v>1996.9742161151501</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>1997</v>
+      </c>
+      <c r="D61">
+        <v>1574.00616675016</v>
+      </c>
+    </row>
+    <row r="62" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62">
+        <v>1997.99798716953</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>1998</v>
+      </c>
+      <c r="D62">
+        <v>1616.7232210337399</v>
+      </c>
+    </row>
+    <row r="63" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B63">
+        <v>1998.97165266149</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>1999</v>
+      </c>
+      <c r="D63">
+        <v>1551.5651873008301</v>
+      </c>
+    </row>
+    <row r="64" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="B64">
+        <v>1999.9441345575001</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="D64">
+        <v>1601.9691593627999</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B65">
+        <v>2000.9956412106001</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>2001</v>
+      </c>
+      <c r="D65">
+        <v>1436.68321118623</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B66">
+        <v>2001.94176836983</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>2002</v>
+      </c>
+      <c r="D66">
+        <v>1560.2678456143201</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B67">
+        <v>2002.99161798859</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>2003</v>
+      </c>
+      <c r="D67">
+        <v>1556.7687055505901</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68">
+        <v>2003.96181159906</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+      <c r="D68">
+        <v>1830.5925554826699</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B69">
+        <v>2004.98672679621</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+      <c r="D69">
+        <v>1761.5996708312</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B70">
+        <v>2005.98741772932</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+      <c r="D70">
+        <v>1557.77583811506</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B71">
+        <v>2006.9870434260599</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+      <c r="D71">
+        <v>1457.9578106143099</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B72">
+        <v>2007.9866296696</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="0"/>
+        <v>2008</v>
+      </c>
+      <c r="D72">
+        <v>1361.9918499733999</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B73">
+        <v>2008.9866498983299</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="0"/>
+        <v>2009</v>
+      </c>
+      <c r="D73">
+        <v>1223.65315387436</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B74">
+        <v>2009.98501309272</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="D74">
+        <v>1247.10126588816</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B75">
+        <v>2011.0108751666301</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="D75">
+        <v>1085.6587766007799</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B76">
+        <v>2011.98544808217</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="D76">
+        <v>931.90320509178696</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{94D15339-5299-4FCA-8354-CF4E87ADBB44}"/>
+    <hyperlink ref="F41" r:id="rId1" xr:uid="{94D15339-5299-4FCA-8354-CF4E87ADBB44}"/>
+    <hyperlink ref="O5" r:id="rId2" xr:uid="{3758DEA6-75C3-45A5-8616-5E109B5F9F23}"/>
+    <hyperlink ref="O7" r:id="rId3" xr:uid="{AB8969BE-A495-4D93-8C92-2B4A1911755D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82504E32-AD8D-4CF2-9245-8E305C2EA8BC}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3593,7 +3729,7 @@
         <v>1109</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3909,6 +4045,20 @@
       </c>
       <c r="D23" s="3" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>2018</v>
+      </c>
+      <c r="B24" s="1">
+        <v>7120</v>
+      </c>
+      <c r="C24" s="10">
+        <v>835</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3935,38 +4085,45 @@
     <hyperlink ref="D8" r:id="rId20" xr:uid="{CD27E74A-65A1-43D6-A3DD-26C2315E165C}"/>
     <hyperlink ref="K3" r:id="rId21" xr:uid="{BE0C280B-578D-4011-A88E-8A4F918B512C}"/>
     <hyperlink ref="D2" r:id="rId22" xr:uid="{F2FD0724-F160-41EF-9AEB-FCEB2A0C41B7}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{812B0837-AC59-443C-8751-2EF604BBB205}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId24"/>
+  <drawing r:id="rId25"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF9E7C2-12AE-4B25-A0D9-44A705B919BC}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
+    <sheetView topLeftCell="A3" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" s="5"/>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3980,7 +4137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3991,7 +4148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>2005</v>
       </c>
@@ -3999,15 +4156,18 @@
         <v>223060</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>2006</v>
       </c>
       <c r="B7" s="1">
         <v>230490</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>2007</v>
       </c>
@@ -4015,7 +4175,7 @@
         <v>263440</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>2008</v>
       </c>
@@ -4023,7 +4183,7 @@
         <v>266640</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>2009</v>
       </c>
@@ -4031,7 +4191,7 @@
         <v>284620</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>2010</v>
       </c>
@@ -4039,7 +4199,7 @@
         <v>273100</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -4047,7 +4207,7 @@
         <v>218010</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>2012</v>
       </c>
@@ -4055,7 +4215,7 @@
         <v>293790</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>2013</v>
       </c>
@@ -4063,7 +4223,7 @@
         <v>272420</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>2014</v>
       </c>
@@ -4071,7 +4231,7 @@
         <v>215010</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>2015</v>
       </c>
@@ -4168,7 +4328,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I7" r:id="rId1" xr:uid="{86141BAD-CC4F-4F91-BDD3-6E3286E4FC59}"/>
+    <hyperlink ref="J1" r:id="rId2" xr:uid="{8562CFD3-9F22-43A1-8C89-C3B28C803A27}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>